<commit_message>
case if user aleady exists
</commit_message>
<xml_diff>
--- a/src/test/java/resource/EmployeeDetails.xlsx
+++ b/src/test/java/resource/EmployeeDetails.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CucumberFramework\Orangehrm\src\test\java\resource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Orangehrm\src\test\java\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40A1A43-16F6-47BC-B802-3641E55123E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DE1414-B28F-45F0-A101-4372ECB2BE3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Raj</t>
   </si>
@@ -40,6 +40,27 @@
   </si>
   <si>
     <t>Rajkumar</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Middle Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>User Name</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Confirm Password</t>
+  </si>
+  <si>
+    <t>Employee id(INT  only )</t>
   </si>
 </sst>
 </file>
@@ -364,7 +385,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:B7"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
@@ -372,40 +393,62 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="30.77734375" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
       <c r="B4" s="1">
         <v>1012</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>

</xml_diff>